<commit_message>
error logging and messaging updates
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\sql2excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanson\Documents\Dev\GitHub\sql2excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Job</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>WebHookSuccess</t>
-  </si>
-  <si>
-    <t>https://glfhc.webhook.office.com/webhookb2/83d67cc8-4d94-447c-91e1-a49cf8efc9db@158b8843-5b77-4790-b011-e3b82aded516/IncomingWebhook/3ab6046f025e42f0ba103e30d89bf8cf/b80ee9c6-d488-4e96-bd2e-ba30e422d7cd</t>
   </si>
   <si>
     <t>https://glfhc.webhook.office.com/webhookb2/83d67cc8-4d94-447c-91e1-a49cf8efc9db@158b8843-5b77-4790-b011-e3b82aded516/IncomingWebhook/c548c74cadaa468f9f52c21beeca657c/b80ee9c6-d488-4e96-bd2e-ba30e422d7cd</t>
@@ -163,6 +160,12 @@
   </si>
   <si>
     <t>1_Telehealth next 7 days.sql</t>
+  </si>
+  <si>
+    <t>EmailOnError</t>
+  </si>
+  <si>
+    <t>chanson@glfhc.org</t>
   </si>
 </sst>
 </file>
@@ -252,7 +255,26 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -277,7 +299,7 @@
     <tableColumn id="8" name="Email" dataCellStyle="Normal"/>
     <tableColumn id="9" name="EmailSubject"/>
     <tableColumn id="10" name="EmailBody"/>
-    <tableColumn id="6" name="WebHookError"/>
+    <tableColumn id="11" name="EmailOnError" dataDxfId="0" dataCellStyle="Hyperlink"/>
     <tableColumn id="7" name="WebHookSuccess"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -550,7 +572,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +585,7 @@
     <col min="6" max="6" width="29.140625" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" customWidth="1"/>
     <col min="8" max="8" width="86.140625" customWidth="1"/>
-    <col min="9" max="9" width="197.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
     <col min="10" max="10" width="197.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -578,22 +600,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -607,28 +629,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
         <v>6</v>
-      </c>
-      <c r="J2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -639,28 +661,28 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
         <v>6</v>
-      </c>
-      <c r="J3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -693,7 +715,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -701,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -709,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -717,15 +739,15 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -733,17 +755,17 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -751,7 +773,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -759,7 +781,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>